<commit_message>
Useless spaces removed in expected XLSX theme1.xml
Fix #36
</commit_message>
<xml_diff>
--- a/src/zdemo_excel16.w3mi.data.xlsx
+++ b/src/zdemo_excel16.w3mi.data.xlsx
@@ -88,7 +88,7 @@
     <xdr:ext cx="1581150" cy="714375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="0800271CCEE91EDC99E75C9C4624EFEB"/>
+        <xdr:cNvPr id="1" name="000D3AAA88F21EDDBB9D66576389B5A5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -115,7 +115,7 @@
     <xdr:ext cx="790575" cy="1524000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="0800271CCEE91EDC99E75C9C46250FEB"/>
+        <xdr:cNvPr id="2" name="000D3AAA88F21EDDBB9D66576389D5A5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -142,7 +142,7 @@
     <xdr:ext cx="1200150" cy="1381125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="0800271CCEE91EDC99E75C9C46252FEB"/>
+        <xdr:cNvPr id="3" name="000D3AAA88F21EDDBB9D66576389F5A5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>

<commit_message>
Useless spaces removed in expected XLSX theme1.xml (#37)
Fix #36

Co-authored-by: sandraros <sandra.rossi@gmail.com>
</commit_message>
<xml_diff>
--- a/src/zdemo_excel16.w3mi.data.xlsx
+++ b/src/zdemo_excel16.w3mi.data.xlsx
@@ -88,7 +88,7 @@
     <xdr:ext cx="1581150" cy="714375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="0800271CCEE91EDC99E75C9C4624EFEB"/>
+        <xdr:cNvPr id="1" name="000D3AAA88F21EDDBB9D66576389B5A5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -115,7 +115,7 @@
     <xdr:ext cx="790575" cy="1524000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="0800271CCEE91EDC99E75C9C46250FEB"/>
+        <xdr:cNvPr id="2" name="000D3AAA88F21EDDBB9D66576389D5A5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -142,7 +142,7 @@
     <xdr:ext cx="1200150" cy="1381125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="0800271CCEE91EDC99E75C9C46252FEB"/>
+        <xdr:cNvPr id="3" name="000D3AAA88F21EDDBB9D66576389F5A5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>

<commit_message>
zdemo_excel16 dynamic SAP GUI path
</commit_message>
<xml_diff>
--- a/src/zdemo_excel16.w3mi.data.xlsx
+++ b/src/zdemo_excel16.w3mi.data.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Image from a file (c:\Program Files\SAP\FrontEnd\SAPgui\wwi\graphics\W_bio.bmp)</t>
+    <t>Image from a file (&lt;SAPGUI-directory&gt;\wwi\graphics\W_bio.bmp)</t>
   </si>
   <si>
     <t>Image from web repository (SMW0)</t>
@@ -88,7 +88,7 @@
     <xdr:ext cx="1581150" cy="714375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="0242AC1100031EEEBD981717274B5650"/>
+        <xdr:cNvPr id="1" name="1FCB857059FD1EDEBEAEE72CCDB39CB1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -115,7 +115,7 @@
     <xdr:ext cx="790575" cy="1524000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="0242AC1100031EEEBD981717274B7650"/>
+        <xdr:cNvPr id="2" name="1FCB857059FD1EDEBEAEE72CCDB3BCB1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -142,7 +142,7 @@
     <xdr:ext cx="1200150" cy="1381125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="0242AC1100031EEEBD981717274B9650"/>
+        <xdr:cNvPr id="3" name="1FCB857059FD1EDEBEAEE72CCDB3DCB1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>

<commit_message>
fixed missing image (#59)
* fixed missing image
* zdemo_excel16 dynamic SAP GUI path

---------

Co-authored-by: sandraros <sandra.rossi@gmail.com>
</commit_message>
<xml_diff>
--- a/src/zdemo_excel16.w3mi.data.xlsx
+++ b/src/zdemo_excel16.w3mi.data.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Image from a file (c:\Program Files\SAP\FrontEnd\SAPgui\wwi\graphics\W_bio.bmp)</t>
+    <t>Image from a file (&lt;SAPGUI-directory&gt;\wwi\graphics\W_bio.bmp)</t>
   </si>
   <si>
     <t>Image from web repository (SMW0)</t>
@@ -88,7 +88,7 @@
     <xdr:ext cx="1581150" cy="714375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="000D3AAA88F21EDDBB9D66576389B5A5"/>
+        <xdr:cNvPr id="1" name="1FCB857059FD1EDEBEAEE72CCDB39CB1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -115,7 +115,7 @@
     <xdr:ext cx="790575" cy="1524000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="000D3AAA88F21EDDBB9D66576389D5A5"/>
+        <xdr:cNvPr id="2" name="1FCB857059FD1EDEBEAEE72CCDB3BCB1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -142,7 +142,7 @@
     <xdr:ext cx="1200150" cy="1381125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="000D3AAA88F21EDDBB9D66576389F5A5"/>
+        <xdr:cNvPr id="3" name="1FCB857059FD1EDEBEAEE72CCDB3DCB1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>

<commit_message>
Demonstrate a tiny shift of image
IP_ROWOFF and IP_COLOFF:

  lo_drawing->set_position( ip_from_row = 3
                            ip_from_col = 'B'
                            ip_rowoff   = 85725
                            ip_coloff   = 47625 ).
</commit_message>
<xml_diff>
--- a/src/zdemo_excel16.w3mi.data.xlsx
+++ b/src/zdemo_excel16.w3mi.data.xlsx
@@ -81,14 +81,14 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1581150" cy="714375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="1FCB857059FD1EDEBEAEE72CCDB39CB1"/>
+        <xdr:cNvPr id="1" name="3D8034E34B381EDF83EE5F36E6D9DCC2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -115,7 +115,7 @@
     <xdr:ext cx="790575" cy="1524000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="1FCB857059FD1EDEBEAEE72CCDB3BCB1"/>
+        <xdr:cNvPr id="2" name="3D8034E34B381EDF83EE5FC15F3B5CC4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -142,7 +142,7 @@
     <xdr:ext cx="1200150" cy="1381125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="1FCB857059FD1EDEBEAEE72CCDB3DCB1"/>
+        <xdr:cNvPr id="3" name="3D8034E34B381EDF83EE5FC15F3B7CC4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>

<commit_message>
Demonstrate a tiny shift of image (#62)
* Demonstrate a tiny shift of image
</commit_message>
<xml_diff>
--- a/src/zdemo_excel16.w3mi.data.xlsx
+++ b/src/zdemo_excel16.w3mi.data.xlsx
@@ -81,14 +81,14 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1581150" cy="714375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="1FCB857059FD1EDEBEAEE72CCDB39CB1"/>
+        <xdr:cNvPr id="1" name="3D8034E34B381EDF83EE5F36E6D9DCC2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -115,7 +115,7 @@
     <xdr:ext cx="790575" cy="1524000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="1FCB857059FD1EDEBEAEE72CCDB3BCB1"/>
+        <xdr:cNvPr id="2" name="3D8034E34B381EDF83EE5FC15F3B5CC4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -142,7 +142,7 @@
     <xdr:ext cx="1200150" cy="1381125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="1FCB857059FD1EDEBEAEE72CCDB3DCB1"/>
+        <xdr:cNvPr id="3" name="3D8034E34B381EDF83EE5FC15F3B7CC4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>